<commit_message>
Exported gantt and meeting logs to webpages
</commit_message>
<xml_diff>
--- a/docs/gantt_meeting-logs/Gantt.xlsx
+++ b/docs/gantt_meeting-logs/Gantt.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26915"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zach/Repos/BitsPlease-FESP/docs/gantt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zach/Repos/BitsPlease-FESP/docs/gantt_meeting-logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4720" yWindow="3980" windowWidth="19840" windowHeight="15500" tabRatio="415"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="415"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <definedName name="Today" localSheetId="0">TODAY()</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
+  <webPublishing allowPng="1" targetScreenSize="1024x768" codePage="10000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -617,7 +618,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -680,6 +681,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -875,7 +882,7 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1011,9 +1018,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
@@ -1037,12 +1041,6 @@
       <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1072,6 +1070,18 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -1962,7 +1972,7 @@
                   <a14:compatExt spid="_x0000_s6149"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005180000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2301,7 +2311,7 @@
   <dimension ref="A1:BL71"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="57" zoomScalePageLayoutView="57" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+      <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2366,39 +2376,39 @@
       <c r="C2" s="18"/>
       <c r="F2" s="23"/>
       <c r="G2" s="21"/>
-      <c r="I2" s="74" t="s">
+      <c r="I2" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="N2" s="75" t="s">
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="N2" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="75"/>
+      <c r="O2" s="72"/>
+      <c r="P2" s="72"/>
+      <c r="Q2" s="72"/>
       <c r="R2" s="20"/>
-      <c r="S2" s="76" t="s">
+      <c r="S2" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="T2" s="76"/>
-      <c r="U2" s="76"/>
-      <c r="V2" s="76"/>
+      <c r="T2" s="73"/>
+      <c r="U2" s="73"/>
+      <c r="V2" s="73"/>
       <c r="W2" s="20"/>
-      <c r="X2" s="67" t="s">
+      <c r="X2" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="Y2" s="67"/>
-      <c r="Z2" s="67"/>
-      <c r="AA2" s="67"/>
+      <c r="Y2" s="64"/>
+      <c r="Z2" s="64"/>
+      <c r="AA2" s="64"/>
       <c r="AB2" s="20"/>
-      <c r="AC2" s="68" t="s">
+      <c r="AC2" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="AD2" s="68"/>
-      <c r="AE2" s="68"/>
-      <c r="AF2" s="68"/>
+      <c r="AD2" s="65"/>
+      <c r="AE2" s="65"/>
+      <c r="AF2" s="65"/>
     </row>
     <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
@@ -2408,25 +2418,25 @@
         <v>48</v>
       </c>
       <c r="C3" s="19"/>
-      <c r="D3" s="69" t="s">
+      <c r="D3" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="70"/>
-      <c r="F3" s="72">
+      <c r="E3" s="67"/>
+      <c r="F3" s="69">
         <f ca="1">IFERROR(IF(MIN(Milestones[Start])=0,TODAY(),MIN(Milestones[Start])),TODAY())</f>
         <v>43378</v>
       </c>
-      <c r="G3" s="73"/>
+      <c r="G3" s="70"/>
       <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="69" t="s">
+      <c r="D4" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="70"/>
+      <c r="E4" s="67"/>
       <c r="F4" s="45">
         <v>0</v>
       </c>
@@ -2515,13 +2525,13 @@
       <c r="A5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
       <c r="I5" s="49">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
         <v>43378</v>
@@ -6168,7 +6178,7 @@
         <v>76</v>
       </c>
       <c r="E22" s="31">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F22" s="32">
         <v>43389</v>
@@ -6738,7 +6748,7 @@
         <v>35</v>
       </c>
       <c r="E25" s="31">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="F25" s="32">
         <v>43390</v>
@@ -7666,7 +7676,7 @@
     </row>
     <row r="31" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="14"/>
-      <c r="B31" s="63" t="s">
+      <c r="B31" s="62" t="s">
         <v>58</v>
       </c>
       <c r="C31" s="34" t="s">
@@ -8414,7 +8424,7 @@
         <v>77</v>
       </c>
       <c r="E34" s="31">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="F34" s="32">
         <v>43423</v>
@@ -8650,7 +8660,7 @@
     </row>
     <row r="35" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="14"/>
-      <c r="B35" s="63" t="s">
+      <c r="B35" s="62" t="s">
         <v>67</v>
       </c>
       <c r="C35" s="34" t="s">
@@ -8906,7 +8916,7 @@
         <v>77</v>
       </c>
       <c r="E36" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36" s="32">
         <v>43395</v>
@@ -9142,7 +9152,7 @@
     </row>
     <row r="37" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="14"/>
-      <c r="B37" s="63" t="s">
+      <c r="B37" s="62" t="s">
         <v>68</v>
       </c>
       <c r="C37" s="34" t="s">
@@ -9388,7 +9398,7 @@
     </row>
     <row r="38" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="14"/>
-      <c r="B38" s="64" t="s">
+      <c r="B38" s="63" t="s">
         <v>69</v>
       </c>
       <c r="C38" s="34"/>
@@ -9626,7 +9636,7 @@
     </row>
     <row r="39" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="14"/>
-      <c r="B39" s="64" t="s">
+      <c r="B39" s="63" t="s">
         <v>79</v>
       </c>
       <c r="C39" s="34" t="s">
@@ -9872,7 +9882,7 @@
     </row>
     <row r="40" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="14"/>
-      <c r="B40" s="64" t="s">
+      <c r="B40" s="63" t="s">
         <v>80</v>
       </c>
       <c r="C40" s="34" t="s">
@@ -10118,7 +10128,7 @@
     </row>
     <row r="41" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="14"/>
-      <c r="B41" s="41" t="s">
+      <c r="B41" s="62" t="s">
         <v>81</v>
       </c>
       <c r="C41" s="34" t="s">
@@ -10362,9 +10372,9 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:64" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="56"/>
-      <c r="B42" s="41" t="s">
+    <row r="42" spans="1:64" s="58" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="55"/>
+      <c r="B42" s="62" t="s">
         <v>82</v>
       </c>
       <c r="C42" s="34" t="s">
@@ -10374,15 +10384,15 @@
         <v>36</v>
       </c>
       <c r="E42" s="30">
-        <v>0</v>
-      </c>
-      <c r="F42" s="60">
+        <v>1</v>
+      </c>
+      <c r="F42" s="59">
         <v>43395</v>
       </c>
-      <c r="G42" s="57">
+      <c r="G42" s="56">
         <v>28</v>
       </c>
-      <c r="H42" s="58"/>
+      <c r="H42" s="57"/>
       <c r="I42" s="38" t="str">
         <f t="shared" ca="1" si="11"/>
         <v/>
@@ -10608,9 +10618,9 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:64" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="56"/>
-      <c r="B43" s="63" t="s">
+    <row r="43" spans="1:64" s="58" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="55"/>
+      <c r="B43" s="62" t="s">
         <v>87</v>
       </c>
       <c r="C43" s="34" t="s">
@@ -10628,7 +10638,7 @@
       <c r="G43" s="33">
         <v>7</v>
       </c>
-      <c r="H43" s="58"/>
+      <c r="H43" s="57"/>
       <c r="I43" s="38" t="str">
         <f t="shared" ca="1" si="11"/>
         <v/>
@@ -11326,7 +11336,7 @@
     </row>
     <row r="46" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="14"/>
-      <c r="B46" s="63" t="s">
+      <c r="B46" s="62" t="s">
         <v>58</v>
       </c>
       <c r="C46" s="34" t="s">
@@ -11336,7 +11346,7 @@
         <v>86</v>
       </c>
       <c r="E46" s="31">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F46" s="32">
         <v>43395</v>
@@ -11572,7 +11582,7 @@
     </row>
     <row r="47" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="14"/>
-      <c r="B47" s="41" t="s">
+      <c r="B47" s="74" t="s">
         <v>59</v>
       </c>
       <c r="C47" s="34" t="s">
@@ -11810,7 +11820,7 @@
     </row>
     <row r="48" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="14"/>
-      <c r="B48" s="55" t="s">
+      <c r="B48" s="63" t="s">
         <v>60</v>
       </c>
       <c r="C48" s="34" t="s">
@@ -12056,7 +12066,7 @@
     </row>
     <row r="49" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="14"/>
-      <c r="B49" s="64" t="s">
+      <c r="B49" s="63" t="s">
         <v>61</v>
       </c>
       <c r="C49" s="34" t="s">
@@ -12302,7 +12312,7 @@
     </row>
     <row r="50" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="14"/>
-      <c r="B50" s="63" t="s">
+      <c r="B50" s="62" t="s">
         <v>62</v>
       </c>
       <c r="C50" s="34" t="s">
@@ -12548,7 +12558,7 @@
     </row>
     <row r="51" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="14"/>
-      <c r="B51" s="41" t="s">
+      <c r="B51" s="74" t="s">
         <v>63</v>
       </c>
       <c r="C51" s="34" t="s">
@@ -12794,7 +12804,7 @@
     </row>
     <row r="52" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="14"/>
-      <c r="B52" s="63" t="s">
+      <c r="B52" s="62" t="s">
         <v>67</v>
       </c>
       <c r="C52" s="34" t="s">
@@ -13040,7 +13050,7 @@
     </row>
     <row r="53" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="14"/>
-      <c r="B53" s="65" t="s">
+      <c r="B53" s="75" t="s">
         <v>71</v>
       </c>
       <c r="C53" s="34" t="s">
@@ -13286,7 +13296,7 @@
     </row>
     <row r="54" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="14"/>
-      <c r="B54" s="66" t="s">
+      <c r="B54" s="76" t="s">
         <v>72</v>
       </c>
       <c r="C54" s="34" t="s">
@@ -13530,7 +13540,7 @@
     </row>
     <row r="55" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="14"/>
-      <c r="B55" s="65" t="s">
+      <c r="B55" s="75" t="s">
         <v>70</v>
       </c>
       <c r="C55" s="34" t="s">
@@ -13776,7 +13786,7 @@
     </row>
     <row r="56" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="14"/>
-      <c r="B56" s="65" t="s">
+      <c r="B56" s="75" t="s">
         <v>69</v>
       </c>
       <c r="C56" s="34" t="s">
@@ -14966,7 +14976,7 @@
     </row>
     <row r="61" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="14"/>
-      <c r="B61" s="64" t="s">
+      <c r="B61" s="63" t="s">
         <v>91</v>
       </c>
       <c r="C61" s="34" t="s">
@@ -15212,7 +15222,7 @@
     </row>
     <row r="62" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="14"/>
-      <c r="B62" s="64" t="s">
+      <c r="B62" s="63" t="s">
         <v>92</v>
       </c>
       <c r="C62" s="34" t="s">
@@ -15458,7 +15468,7 @@
     </row>
     <row r="63" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="14"/>
-      <c r="B63" s="55" t="s">
+      <c r="B63" s="77" t="s">
         <v>93</v>
       </c>
       <c r="C63" s="34" t="s">
@@ -15704,7 +15714,7 @@
     </row>
     <row r="64" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="14"/>
-      <c r="B64" s="63" t="s">
+      <c r="B64" s="62" t="s">
         <v>97</v>
       </c>
       <c r="C64" s="34" t="s">
@@ -15782,7 +15792,7 @@
     </row>
     <row r="65" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="14"/>
-      <c r="B65" s="63" t="s">
+      <c r="B65" s="62" t="s">
         <v>94</v>
       </c>
       <c r="C65" s="34"/>
@@ -15850,7 +15860,7 @@
     </row>
     <row r="66" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="14"/>
-      <c r="B66" s="64" t="s">
+      <c r="B66" s="63" t="s">
         <v>95</v>
       </c>
       <c r="C66" s="34" t="s">
@@ -15928,7 +15938,7 @@
     </row>
     <row r="67" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="14"/>
-      <c r="B67" s="64" t="s">
+      <c r="B67" s="63" t="s">
         <v>96</v>
       </c>
       <c r="C67" s="34" t="s">
@@ -17007,7 +17017,7 @@
       <c r="C2" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="60" t="s">
         <v>98</v>
       </c>
     </row>
@@ -17021,7 +17031,7 @@
       <c r="C3" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="60" t="s">
         <v>99</v>
       </c>
     </row>
@@ -17035,7 +17045,7 @@
       <c r="C4" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="61" t="s">
+      <c r="D4" s="60" t="s">
         <v>101</v>
       </c>
     </row>
@@ -17049,7 +17059,7 @@
       <c r="C5" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="61" t="s">
+      <c r="D5" s="60" t="s">
         <v>104</v>
       </c>
     </row>
@@ -17063,7 +17073,7 @@
       <c r="C6" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="61" t="s">
+      <c r="D6" s="60" t="s">
         <v>103</v>
       </c>
     </row>
@@ -17077,7 +17087,7 @@
       <c r="C7" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="D7" s="61" t="s">
+      <c r="D7" s="60" t="s">
         <v>105</v>
       </c>
     </row>
@@ -17091,7 +17101,7 @@
       <c r="C8" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="61" t="s">
+      <c r="D8" s="60" t="s">
         <v>106</v>
       </c>
     </row>
@@ -17105,7 +17115,7 @@
       <c r="C9" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="D9" s="61" t="s">
+      <c r="D9" s="60" t="s">
         <v>107</v>
       </c>
     </row>
@@ -17119,12 +17129,12 @@
       <c r="C10" t="s">
         <v>108</v>
       </c>
-      <c r="D10" s="61" t="s">
+      <c r="D10" s="60" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="62">
+      <c r="A11" s="61">
         <v>43402</v>
       </c>
       <c r="B11" t="s">
@@ -17133,23 +17143,23 @@
       <c r="C11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="61" t="s">
+      <c r="D11" s="60" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="62">
+      <c r="A12" s="61">
         <v>43404</v>
       </c>
       <c r="C12" t="s">
         <v>108</v>
       </c>
-      <c r="D12" s="61" t="s">
+      <c r="D12" s="60" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="62">
+      <c r="A13" s="61">
         <v>43407</v>
       </c>
       <c r="B13" t="s">
@@ -17158,12 +17168,12 @@
       <c r="C13" t="s">
         <v>112</v>
       </c>
-      <c r="D13" s="61" t="s">
+      <c r="D13" s="60" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="62">
+      <c r="A14" s="61">
         <v>43411</v>
       </c>
       <c r="B14" t="s">
@@ -17172,12 +17182,12 @@
       <c r="C14" t="s">
         <v>114</v>
       </c>
-      <c r="D14" s="61" t="s">
+      <c r="D14" s="60" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="62">
+      <c r="A15" s="61">
         <v>43413</v>
       </c>
       <c r="B15" t="s">
@@ -17186,12 +17196,12 @@
       <c r="C15" t="s">
         <v>114</v>
       </c>
-      <c r="D15" s="61" t="s">
+      <c r="D15" s="60" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A16" s="62">
+      <c r="A16" s="61">
         <v>43414</v>
       </c>
       <c r="B16" t="s">
@@ -17200,12 +17210,12 @@
       <c r="C16" t="s">
         <v>114</v>
       </c>
-      <c r="D16" s="61" t="s">
+      <c r="D16" s="60" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="62">
+      <c r="A17" s="61">
         <v>43416</v>
       </c>
       <c r="B17" t="s">
@@ -17214,12 +17224,12 @@
       <c r="C17" t="s">
         <v>108</v>
       </c>
-      <c r="D17" s="61" t="s">
+      <c r="D17" s="60" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A18" s="62">
+      <c r="A18" s="61">
         <v>43417</v>
       </c>
       <c r="B18" t="s">
@@ -17228,12 +17238,12 @@
       <c r="C18" t="s">
         <v>119</v>
       </c>
-      <c r="D18" s="61" t="s">
+      <c r="D18" s="60" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="62">
+      <c r="A19" s="61">
         <v>43418</v>
       </c>
       <c r="B19" t="s">
@@ -17242,12 +17252,12 @@
       <c r="C19" t="s">
         <v>114</v>
       </c>
-      <c r="D19" s="61" t="s">
+      <c r="D19" s="60" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="62">
+      <c r="A20" s="61">
         <v>43420</v>
       </c>
       <c r="B20" t="s">
@@ -17256,12 +17266,12 @@
       <c r="C20" t="s">
         <v>108</v>
       </c>
-      <c r="D20" s="61" t="s">
+      <c r="D20" s="60" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="62">
+      <c r="A21" s="61">
         <v>43423</v>
       </c>
       <c r="B21" t="s">
@@ -17270,12 +17280,12 @@
       <c r="C21" t="s">
         <v>108</v>
       </c>
-      <c r="D21" s="61" t="s">
+      <c r="D21" s="60" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="62">
+      <c r="A22" s="61">
         <v>43427</v>
       </c>
       <c r="B22" t="s">
@@ -17284,12 +17294,12 @@
       <c r="C22" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="61" t="s">
+      <c r="D22" s="60" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="62">
+      <c r="A23" s="61">
         <v>43428</v>
       </c>
       <c r="B23" t="s">
@@ -17298,12 +17308,12 @@
       <c r="C23" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="61" t="s">
+      <c r="D23" s="60" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="62">
+      <c r="A24" s="61">
         <v>43429</v>
       </c>
       <c r="B24" t="s">
@@ -17312,13 +17322,13 @@
       <c r="C24" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="61" t="s">
+      <c r="D24" s="60" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="62"/>
-      <c r="D25" s="61"/>
+      <c r="A25" s="61"/>
+      <c r="D25" s="60"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated to reflect current project 4 status
</commit_message>
<xml_diff>
--- a/docs/gantt_meeting-logs/Gantt.xlsx
+++ b/docs/gantt_meeting-logs/Gantt.xlsx
@@ -1,15 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" checkCompatibility="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zach/Repos/BitsPlease-FESP/docs/gantt_meeting-logs/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA37BDF-60C4-4A33-AFB4-4791C1C6F0BC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="415"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="20535" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -22,29 +18,30 @@
     <definedName name="Scrolling_Increment">Gantt!$F$4</definedName>
     <definedName name="Today" localSheetId="0">TODAY()</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <webPublishing allowPng="1" targetScreenSize="1024x768" codePage="10000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="128">
   <si>
     <t>About This Template</t>
   </si>
@@ -322,9 +319,6 @@
     <t xml:space="preserve">       HUD</t>
   </si>
   <si>
-    <t>Thomas/Gage</t>
-  </si>
-  <si>
     <t>Physics/ Backend</t>
   </si>
   <si>
@@ -460,7 +454,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="d"/>
@@ -618,7 +612,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -680,13 +674,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1037,12 +1025,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1071,24 +1053,30 @@
     <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="3"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Accent3" xfId="11" builtinId="37"/>
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
     <cellStyle name="Comma [0]" xfId="10" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Date" xfId="9"/>
+    <cellStyle name="Date" xfId="9" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="7" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
@@ -1096,14 +1084,14 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5" customBuiltin="1"/>
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="zHiddenText" xfId="3"/>
+    <cellStyle name="zHiddenText" xfId="3" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
   </cellStyles>
   <dxfs count="47">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+      <numFmt numFmtId="165" formatCode="m/d/yy"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1836,12 +1824,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Gantt Table Style" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Gantt Table Style" pivot="0" count="3">
+    <tableStyle name="Gantt Table Style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="46"/>
       <tableStyleElement type="headerRow" dxfId="45"/>
       <tableStyleElement type="firstRowStripe" dxfId="44"/>
     </tableStyle>
-    <tableStyle name="ToDoList" pivot="0" count="9">
+    <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="wholeTable" dxfId="43"/>
       <tableStyleElement type="headerRow" dxfId="42"/>
       <tableStyleElement type="totalRow" dxfId="41"/>
@@ -1954,15 +1942,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>25400</xdr:colOff>
+          <xdr:colOff>28575</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>63500</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>63</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
+          <xdr:col>64</xdr:col>
+          <xdr:colOff>6350</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>241300</xdr:rowOff>
+          <xdr:rowOff>238125</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1972,7 +1960,7 @@
                   <a14:compatExt spid="_x0000_s6149"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005180000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2003,8 +1991,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Milestones" displayName="Milestones" ref="B7:G68" totalsRowShown="0">
-  <autoFilter ref="B7:G68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Milestones" displayName="Milestones" ref="B7:G68" totalsRowShown="0">
+  <autoFilter ref="B7:G68" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2013,12 +2001,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" name="Milestone Description" dataDxfId="4"/>
-    <tableColumn id="2" name="Category" dataDxfId="3"/>
-    <tableColumn id="3" name="Assigned To" dataDxfId="2"/>
-    <tableColumn id="4" name="Progress"/>
-    <tableColumn id="5" name="Start" dataCellStyle="Date"/>
-    <tableColumn id="6" name="No. Days" dataCellStyle="Comma [0]"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone Description" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Assigned To" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Progress"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start" dataCellStyle="Date"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No. Days" dataCellStyle="Comma [0]"/>
   </tableColumns>
   <tableStyleInfo name="Gantt Table Style" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2030,13 +2018,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D25" totalsRowShown="0">
-  <autoFilter ref="A1:D25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:D25" totalsRowShown="0">
+  <autoFilter ref="A1:D25" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Date" dataDxfId="1"/>
-    <tableColumn id="2" name="Location"/>
-    <tableColumn id="3" name="Members"/>
-    <tableColumn id="4" name="Things Discussed" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Location"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Members"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Things Discussed" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Gantt Table Style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2304,30 +2292,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BL71"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="57" zoomScalePageLayoutView="57" workbookViewId="0">
-      <selection activeCell="Y16" sqref="Y16"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="20" customWidth="1"/>
-    <col min="4" max="4" width="20.5" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.5" customWidth="1"/>
-    <col min="8" max="8" width="2.6640625" customWidth="1"/>
-    <col min="9" max="64" width="3.5" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" customWidth="1"/>
+    <col min="9" max="64" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
         <v>23</v>
       </c>
@@ -2366,7 +2354,7 @@
       <c r="AF1" s="20"/>
       <c r="AG1" s="20"/>
     </row>
-    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>15</v>
       </c>
@@ -2376,41 +2364,41 @@
       <c r="C2" s="18"/>
       <c r="F2" s="23"/>
       <c r="G2" s="21"/>
-      <c r="I2" s="71" t="s">
+      <c r="I2" s="69" t="s">
         <v>77</v>
       </c>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="N2" s="72" t="s">
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="N2" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="O2" s="72"/>
-      <c r="P2" s="72"/>
-      <c r="Q2" s="72"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
       <c r="R2" s="20"/>
-      <c r="S2" s="73" t="s">
+      <c r="S2" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="T2" s="73"/>
-      <c r="U2" s="73"/>
-      <c r="V2" s="73"/>
+      <c r="T2" s="71"/>
+      <c r="U2" s="71"/>
+      <c r="V2" s="71"/>
       <c r="W2" s="20"/>
-      <c r="X2" s="64" t="s">
+      <c r="X2" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="Y2" s="64"/>
-      <c r="Z2" s="64"/>
-      <c r="AA2" s="64"/>
+      <c r="Y2" s="62"/>
+      <c r="Z2" s="62"/>
+      <c r="AA2" s="62"/>
       <c r="AB2" s="20"/>
-      <c r="AC2" s="65" t="s">
+      <c r="AC2" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="AD2" s="65"/>
-      <c r="AE2" s="65"/>
-      <c r="AF2" s="65"/>
+      <c r="AD2" s="63"/>
+      <c r="AE2" s="63"/>
+      <c r="AF2" s="63"/>
     </row>
-    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
@@ -2418,25 +2406,25 @@
         <v>48</v>
       </c>
       <c r="C3" s="19"/>
-      <c r="D3" s="66" t="s">
+      <c r="D3" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="67"/>
-      <c r="F3" s="69">
+      <c r="E3" s="65"/>
+      <c r="F3" s="67">
         <f ca="1">IFERROR(IF(MIN(Milestones[Start])=0,TODAY(),MIN(Milestones[Start])),TODAY())</f>
         <v>43378</v>
       </c>
-      <c r="G3" s="70"/>
+      <c r="G3" s="68"/>
       <c r="H3" s="22"/>
     </row>
-    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="66" t="s">
+      <c r="D4" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="67"/>
+      <c r="E4" s="65"/>
       <c r="F4" s="45">
         <v>0</v>
       </c>
@@ -2521,17 +2509,17 @@
       <c r="BK4" s="44"/>
       <c r="BL4" s="44"/>
     </row>
-    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
       <c r="I5" s="49">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
         <v>43378</v>
@@ -2757,7 +2745,7 @@
         <v>43433</v>
       </c>
     </row>
-    <row r="6" spans="1:64" s="20" customFormat="1" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:64" s="20" customFormat="1" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>18</v>
       </c>
@@ -2825,7 +2813,7 @@
       <c r="BK6" s="47"/>
       <c r="BL6" s="48"/>
     </row>
-    <row r="7" spans="1:64" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:64" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>19</v>
       </c>
@@ -3073,7 +3061,7 @@
         <v>T</v>
       </c>
     </row>
-    <row r="8" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>25</v>
       </c>
@@ -3140,7 +3128,7 @@
       <c r="BK8" s="36"/>
       <c r="BL8" s="36"/>
     </row>
-    <row r="9" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>20</v>
       </c>
@@ -3384,7 +3372,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
       <c r="B10" s="41" t="s">
         <v>29</v>
@@ -3630,7 +3618,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="B11" s="52" t="s">
         <v>37</v>
@@ -3642,7 +3630,7 @@
         <v>36</v>
       </c>
       <c r="E11" s="31">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F11" s="32">
         <v>43378</v>
@@ -3876,7 +3864,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
       <c r="B12" s="41" t="s">
         <v>30</v>
@@ -4122,7 +4110,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="41" t="s">
         <v>31</v>
@@ -4368,7 +4356,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="41" t="s">
         <v>32</v>
@@ -4380,7 +4368,7 @@
         <v>35</v>
       </c>
       <c r="E14" s="31">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F14" s="32">
         <v>43378</v>
@@ -4614,7 +4602,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="41" t="s">
         <v>33</v>
@@ -4623,10 +4611,10 @@
         <v>43</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E15" s="31">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="F15" s="32">
         <v>43392</v>
@@ -4692,7 +4680,7 @@
       <c r="BK15" s="38"/>
       <c r="BL15" s="38"/>
     </row>
-    <row r="16" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="52" t="s">
         <v>34</v>
@@ -4938,7 +4926,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="42" t="s">
         <v>28</v>
@@ -5182,7 +5170,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="41" t="s">
         <v>38</v>
@@ -5428,7 +5416,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="41" t="s">
         <v>39</v>
@@ -5674,7 +5662,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="41" t="s">
         <v>40</v>
@@ -5920,7 +5908,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="41" t="s">
         <v>41</v>
@@ -6166,7 +6154,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="52" t="s">
         <v>83</v>
@@ -6244,7 +6232,7 @@
       <c r="BK22" s="38"/>
       <c r="BL22" s="38"/>
     </row>
-    <row r="23" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="41" t="s">
         <v>42</v>
@@ -6490,7 +6478,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="52" t="s">
         <v>49</v>
@@ -6736,9 +6724,9 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
-      <c r="B25" s="52" t="s">
+      <c r="B25" s="77" t="s">
         <v>50</v>
       </c>
       <c r="C25" s="34" t="s">
@@ -6814,7 +6802,7 @@
       <c r="BK25" s="38"/>
       <c r="BL25" s="38"/>
     </row>
-    <row r="26" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="41" t="s">
         <v>73</v>
@@ -6892,7 +6880,7 @@
       <c r="BK26" s="38"/>
       <c r="BL26" s="38"/>
     </row>
-    <row r="27" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="41" t="s">
         <v>74</v>
@@ -6970,7 +6958,7 @@
       <c r="BK27" s="38"/>
       <c r="BL27" s="38"/>
     </row>
-    <row r="28" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="52"/>
       <c r="C28" s="34"/>
@@ -7204,7 +7192,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="41"/>
       <c r="C29" s="34"/>
@@ -7438,7 +7426,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="42" t="s">
         <v>64</v>
@@ -7674,9 +7662,9 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
-      <c r="B31" s="62" t="s">
+      <c r="B31" s="72" t="s">
         <v>58</v>
       </c>
       <c r="C31" s="34" t="s">
@@ -7686,7 +7674,7 @@
         <v>44</v>
       </c>
       <c r="E31" s="31">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F31" s="32">
         <v>43395</v>
@@ -7920,7 +7908,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="41" t="s">
         <v>62</v>
@@ -7929,7 +7917,7 @@
         <v>35</v>
       </c>
       <c r="D32" s="34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E32" s="31">
         <v>1</v>
@@ -8166,9 +8154,9 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
-      <c r="B33" s="41" t="s">
+      <c r="B33" s="76" t="s">
         <v>65</v>
       </c>
       <c r="C33" s="34" t="s">
@@ -8412,7 +8400,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="41" t="s">
         <v>66</v>
@@ -8658,9 +8646,9 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14"/>
-      <c r="B35" s="62" t="s">
+      <c r="B35" s="72" t="s">
         <v>67</v>
       </c>
       <c r="C35" s="34" t="s">
@@ -8904,9 +8892,9 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
-      <c r="B36" s="41" t="s">
+      <c r="B36" s="72" t="s">
         <v>70</v>
       </c>
       <c r="C36" s="34" t="s">
@@ -9150,16 +9138,16 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
-      <c r="B37" s="62" t="s">
+      <c r="B37" s="72" t="s">
         <v>68</v>
       </c>
       <c r="C37" s="34" t="s">
         <v>44</v>
       </c>
       <c r="D37" s="34" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="E37" s="31">
         <v>1</v>
@@ -9396,9 +9384,9 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
-      <c r="B38" s="63" t="s">
+      <c r="B38" s="75" t="s">
         <v>69</v>
       </c>
       <c r="C38" s="34"/>
@@ -9634,9 +9622,9 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="14"/>
-      <c r="B39" s="63" t="s">
+      <c r="B39" s="73" t="s">
         <v>79</v>
       </c>
       <c r="C39" s="34" t="s">
@@ -9880,9 +9868,9 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="14"/>
-      <c r="B40" s="63" t="s">
+      <c r="B40" s="73" t="s">
         <v>80</v>
       </c>
       <c r="C40" s="34" t="s">
@@ -10126,9 +10114,9 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="14"/>
-      <c r="B41" s="62" t="s">
+      <c r="B41" s="72" t="s">
         <v>81</v>
       </c>
       <c r="C41" s="34" t="s">
@@ -10372,9 +10360,9 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:64" s="58" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:64" s="58" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="55"/>
-      <c r="B42" s="62" t="s">
+      <c r="B42" s="72" t="s">
         <v>82</v>
       </c>
       <c r="C42" s="34" t="s">
@@ -10618,10 +10606,10 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:64" s="58" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:64" s="58" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="55"/>
-      <c r="B43" s="62" t="s">
-        <v>87</v>
+      <c r="B43" s="72" t="s">
+        <v>86</v>
       </c>
       <c r="C43" s="34" t="s">
         <v>44</v>
@@ -10864,7 +10852,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="41"/>
       <c r="C44" s="34"/>
@@ -11098,10 +11086,10 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="14"/>
       <c r="B45" s="42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C45" s="34"/>
       <c r="D45" s="34"/>
@@ -11334,16 +11322,16 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="14"/>
-      <c r="B46" s="62" t="s">
+      <c r="B46" s="72" t="s">
         <v>58</v>
       </c>
       <c r="C46" s="34" t="s">
         <v>77</v>
       </c>
       <c r="D46" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E46" s="31">
         <v>1</v>
@@ -11580,7 +11568,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14"/>
       <c r="B47" s="74" t="s">
         <v>59</v>
@@ -11818,9 +11806,9 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="14"/>
-      <c r="B48" s="63" t="s">
+      <c r="B48" s="73" t="s">
         <v>60</v>
       </c>
       <c r="C48" s="34" t="s">
@@ -12064,9 +12052,9 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
-      <c r="B49" s="63" t="s">
+      <c r="B49" s="73" t="s">
         <v>61</v>
       </c>
       <c r="C49" s="34" t="s">
@@ -12310,9 +12298,9 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14"/>
-      <c r="B50" s="62" t="s">
+      <c r="B50" s="72" t="s">
         <v>62</v>
       </c>
       <c r="C50" s="34" t="s">
@@ -12556,7 +12544,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="74" t="s">
         <v>63</v>
@@ -12802,9 +12790,9 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="14"/>
-      <c r="B52" s="62" t="s">
+      <c r="B52" s="72" t="s">
         <v>67</v>
       </c>
       <c r="C52" s="34" t="s">
@@ -13048,9 +13036,9 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="14"/>
-      <c r="B53" s="75" t="s">
+      <c r="B53" s="74" t="s">
         <v>71</v>
       </c>
       <c r="C53" s="34" t="s">
@@ -13294,9 +13282,9 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="14"/>
-      <c r="B54" s="76" t="s">
+      <c r="B54" s="75" t="s">
         <v>72</v>
       </c>
       <c r="C54" s="34" t="s">
@@ -13538,9 +13526,9 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="14"/>
-      <c r="B55" s="75" t="s">
+      <c r="B55" s="72" t="s">
         <v>70</v>
       </c>
       <c r="C55" s="34" t="s">
@@ -13550,7 +13538,7 @@
         <v>77</v>
       </c>
       <c r="E55" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F55" s="32">
         <v>43395</v>
@@ -13784,16 +13772,16 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:64" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:64" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="14"/>
-      <c r="B56" s="75" t="s">
+      <c r="B56" s="74" t="s">
         <v>69</v>
       </c>
       <c r="C56" s="34" t="s">
         <v>35</v>
       </c>
       <c r="D56" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E56" s="31">
         <v>0</v>
@@ -14030,7 +14018,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
         <v>2</v>
       </c>
@@ -14266,7 +14254,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
         <v>2</v>
       </c>
@@ -14502,10 +14490,10 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="14"/>
       <c r="B59" s="42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C59" s="34"/>
       <c r="D59" s="34"/>
@@ -14738,10 +14726,10 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="14"/>
       <c r="B60" s="41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C60" s="34"/>
       <c r="D60" s="34"/>
@@ -14974,10 +14962,10 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="14"/>
-      <c r="B61" s="63" t="s">
-        <v>91</v>
+      <c r="B61" s="73" t="s">
+        <v>90</v>
       </c>
       <c r="C61" s="34" t="s">
         <v>77</v>
@@ -15220,10 +15208,10 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="14"/>
-      <c r="B62" s="63" t="s">
-        <v>92</v>
+      <c r="B62" s="73" t="s">
+        <v>91</v>
       </c>
       <c r="C62" s="34" t="s">
         <v>35</v>
@@ -15466,10 +15454,10 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="14"/>
-      <c r="B63" s="77" t="s">
-        <v>93</v>
+      <c r="B63" s="75" t="s">
+        <v>92</v>
       </c>
       <c r="C63" s="34" t="s">
         <v>43</v>
@@ -15712,10 +15700,10 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="14"/>
-      <c r="B64" s="62" t="s">
-        <v>97</v>
+      <c r="B64" s="72" t="s">
+        <v>96</v>
       </c>
       <c r="C64" s="34" t="s">
         <v>44</v>
@@ -15790,10 +15778,10 @@
       <c r="BK64" s="38"/>
       <c r="BL64" s="38"/>
     </row>
-    <row r="65" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="14"/>
-      <c r="B65" s="62" t="s">
-        <v>94</v>
+      <c r="B65" s="72" t="s">
+        <v>93</v>
       </c>
       <c r="C65" s="34"/>
       <c r="D65" s="34"/>
@@ -15858,10 +15846,10 @@
       <c r="BK65" s="38"/>
       <c r="BL65" s="38"/>
     </row>
-    <row r="66" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="14"/>
-      <c r="B66" s="63" t="s">
-        <v>95</v>
+      <c r="B66" s="73" t="s">
+        <v>94</v>
       </c>
       <c r="C66" s="34" t="s">
         <v>77</v>
@@ -15936,10 +15924,10 @@
       <c r="BK66" s="38"/>
       <c r="BL66" s="38"/>
     </row>
-    <row r="67" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="14"/>
-      <c r="B67" s="63" t="s">
-        <v>96</v>
+      <c r="B67" s="73" t="s">
+        <v>95</v>
       </c>
       <c r="C67" s="34" t="s">
         <v>35</v>
@@ -16014,7 +16002,7 @@
       <c r="BK67" s="38"/>
       <c r="BL67" s="38"/>
     </row>
-    <row r="68" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
         <v>2</v>
       </c>
@@ -16250,7 +16238,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="15" t="s">
         <v>26</v>
       </c>
@@ -16320,12 +16308,12 @@
       <c r="BK69" s="37"/>
       <c r="BL69" s="37"/>
     </row>
-    <row r="70" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D70" s="5"/>
       <c r="G70" s="16"/>
       <c r="H70" s="4"/>
     </row>
-    <row r="71" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D71" s="6"/>
     </row>
   </sheetData>
@@ -16565,16 +16553,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Scrolling Increment" prompt="Changing this number will scroll the Gantt Chart view." sqref="F4">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Scrolling Increment" prompt="Changing this number will scroll the Gantt Chart view." sqref="F4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Goal,Milestone,On Track, Low Risk, Med Risk, High Risk"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Jacob,Thomas,Gage,Zach,Goal,Milestone"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C68">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C68" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"Jacob,Thomas,Gage,Zach,Goal,Milestone"</formula1>
     </dataValidation>
   </dataValidations>
@@ -16596,25 +16584,23 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
-                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:colOff>28575</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>63500</xdr:rowOff>
+                    <xdr:rowOff>66675</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>63</xdr:col>
                     <xdr:colOff>228600</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>241300</xdr:rowOff>
+                    <xdr:rowOff>238125</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
-    <mc:Fallback/>
   </mc:AlternateContent>
   <tableParts count="1">
     <tablePart r:id="rId5"/>
@@ -16981,19 +16967,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17" defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="50.5" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -17007,7 +16993,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="54">
         <v>43378</v>
       </c>
@@ -17018,10 +17004,10 @@
         <v>36</v>
       </c>
       <c r="D2" s="60" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="54">
         <v>43383</v>
       </c>
@@ -17032,10 +17018,10 @@
         <v>36</v>
       </c>
       <c r="D3" s="60" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="54">
         <v>43385</v>
       </c>
@@ -17046,38 +17032,38 @@
         <v>36</v>
       </c>
       <c r="D4" s="60" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="54">
         <v>43388</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D5" s="60" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="54">
         <v>43389</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="60" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="54">
         <v>43390</v>
       </c>
@@ -17085,13 +17071,13 @@
         <v>57</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D7" s="60" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="54">
         <v>43392</v>
       </c>
@@ -17102,10 +17088,10 @@
         <v>36</v>
       </c>
       <c r="D8" s="60" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="54">
         <v>43397</v>
       </c>
@@ -17113,13 +17099,13 @@
         <v>57</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D9" s="60" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="54">
         <v>43399</v>
       </c>
@@ -17127,52 +17113,52 @@
         <v>57</v>
       </c>
       <c r="C10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="D10" s="60" t="s">
-        <v>109</v>
-      </c>
     </row>
-    <row r="11" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="61">
         <v>43402</v>
       </c>
       <c r="B11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C11" t="s">
         <v>36</v>
       </c>
       <c r="D11" s="60" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="61">
         <v>43404</v>
       </c>
       <c r="C12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D12" s="60" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="61">
         <v>43407</v>
       </c>
       <c r="B13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="D13" s="60" t="s">
-        <v>113</v>
-      </c>
     </row>
-    <row r="14" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="61">
         <v>43411</v>
       </c>
@@ -17180,13 +17166,13 @@
         <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D14" s="60" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="61">
         <v>43413</v>
       </c>
@@ -17194,55 +17180,55 @@
         <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D15" s="60" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="61">
         <v>43414</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" s="60" t="s">
         <v>114</v>
       </c>
-      <c r="D16" s="60" t="s">
-        <v>115</v>
-      </c>
     </row>
-    <row r="17" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="61">
         <v>43416</v>
       </c>
       <c r="B17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D17" s="60" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="61">
         <v>43417</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D18" s="60" t="s">
         <v>119</v>
       </c>
-      <c r="D18" s="60" t="s">
-        <v>120</v>
-      </c>
     </row>
-    <row r="19" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="61">
         <v>43418</v>
       </c>
@@ -17250,27 +17236,27 @@
         <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D19" s="60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="61">
         <v>43420</v>
       </c>
       <c r="B20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D20" s="60" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="61">
         <v>43423</v>
       </c>
@@ -17278,55 +17264,55 @@
         <v>57</v>
       </c>
       <c r="C21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D21" s="60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="61">
         <v>43427</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D22" s="60" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="61">
         <v>43428</v>
       </c>
       <c r="B23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C23" t="s">
         <v>36</v>
       </c>
       <c r="D23" s="60" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="61">
         <v>43429</v>
       </c>
       <c r="B24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C24" t="s">
         <v>36</v>
       </c>
       <c r="D24" s="60" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="61"/>
       <c r="D25" s="60"/>
     </row>
@@ -17340,25 +17326,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="87.1640625" style="10" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="8"/>
+    <col min="1" max="1" width="87.140625" style="10" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" s="9" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="84.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="84.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>21</v>
       </c>
@@ -17368,7 +17354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="10" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" s="10" customFormat="1" ht="204.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>27</v>
       </c>

</xml_diff>